<commit_message>
Adding changes to landing page
</commit_message>
<xml_diff>
--- a/W2/W02 Assignment - Personal and Team Plan.xlsx
+++ b/W2/W02 Assignment - Personal and Team Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70009505af99092e/Documents/BYU-I Online/ACIT 261 Mobile Application Development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70009505af99092e/Documents/BYU-I Online/ACIT 261 Mobile Application Development/W2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9F6F1E6-8D8B-4091-B648-68D9A6E1ED1C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9F6F1E6-8D8B-4091-B648-68D9A6E1ED1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{76E88BA8-0A9C-4F31-B904-5F1527BCEA8C}"/>
   </bookViews>
@@ -812,15 +812,18 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -829,9 +832,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -964,17 +964,17 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thick">
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <bottom style="thin">
           <color theme="0"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <bottom style="thin">
+        <bottom style="thick">
           <color theme="0"/>
         </bottom>
       </border>
@@ -993,7 +993,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B460820-0B63-4701-87CF-BE905B54702A}" name="Table2" displayName="Table2" ref="A2:C15" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B460820-0B63-4701-87CF-BE905B54702A}" name="Table2" displayName="Table2" ref="A2:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A2:C15" xr:uid="{83FB1169-3128-4809-9FD0-CBF06753023B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{18169B74-9A36-434B-8AB4-63ECC0E35A60}" name="Code Topics" dataDxfId="2"/>
@@ -1541,11 +1541,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="23" t="s">
@@ -1565,7 +1565,7 @@
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -1574,7 +1574,7 @@
       <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="26" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
       <c r="B5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
@@ -1594,7 +1594,7 @@
       <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       <c r="B7" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="24"/>
     </row>
     <row r="8" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
@@ -1614,7 +1614,7 @@
       <c r="B8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
@@ -1623,7 +1623,7 @@
       <c r="B9" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="25"/>
+      <c r="C9" s="24"/>
     </row>
     <row r="10" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
@@ -1632,7 +1632,7 @@
       <c r="B10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="24"/>
     </row>
     <row r="11" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
@@ -1641,7 +1641,7 @@
       <c r="B11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="24"/>
     </row>
     <row r="12" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
@@ -1650,7 +1650,7 @@
       <c r="B12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="24"/>
     </row>
     <row r="13" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
@@ -1659,7 +1659,7 @@
       <c r="B13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
@@ -1668,28 +1668,28 @@
       <c r="B14" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="24"/>
     </row>
     <row r="15" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
     </row>
     <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Section 3 fixing landing
</commit_message>
<xml_diff>
--- a/W2/W02 Assignment - Personal and Team Plan.xlsx
+++ b/W2/W02 Assignment - Personal and Team Plan.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{C9F6F1E6-8D8B-4091-B648-68D9A6E1ED1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{76E88BA8-0A9C-4F31-B904-5F1527BCEA8C}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7995" activeTab="1" xr2:uid="{76E88BA8-0A9C-4F31-B904-5F1527BCEA8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Plan" sheetId="1" r:id="rId1"/>
@@ -1529,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922FE3FC-8426-410B-802B-219C9F87BA40}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final Project Revision 1.1
</commit_message>
<xml_diff>
--- a/W2/W02 Assignment - Personal and Team Plan.xlsx
+++ b/W2/W02 Assignment - Personal and Team Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{C9F6F1E6-8D8B-4091-B648-68D9A6E1ED1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7995" activeTab="1" xr2:uid="{76E88BA8-0A9C-4F31-B904-5F1527BCEA8C}"/>
+    <workbookView xWindow="8850" yWindow="1635" windowWidth="19020" windowHeight="10875" activeTab="1" xr2:uid="{76E88BA8-0A9C-4F31-B904-5F1527BCEA8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Plan" sheetId="1" r:id="rId1"/>
@@ -1530,7 +1530,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>